<commit_message>
Converted alcohol to units, changed MET threshold from 150 to 600, generalised outcome variable in regressiontable function and made correlation matrix for Townsend/education/income/employment
</commit_message>
<xml_diff>
--- a/Data Management/DataDictionary/DataDictionary.xlsx
+++ b/Data Management/DataDictionary/DataDictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TEU\APOE on Dementia\Data Management\DataDictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Kdrive\ukb_hypertension\Data Management\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="167">
   <si>
     <t>age</t>
   </si>
@@ -147,12 +147,6 @@
     <t>There are 88 non-cancer illness codes categorised as other chronic co-morbidities, probably don't want to list them all here?</t>
   </si>
   <si>
-    <t>An indicator variable for whether the participant's average daily METs exceeded 150</t>
-  </si>
-  <si>
-    <t>The summed MET minutes per week were divided by 7 to get average daily METs</t>
-  </si>
-  <si>
     <t>UKBfield</t>
   </si>
   <si>
@@ -468,15 +462,9 @@
     <t>HTNdx_durcat</t>
   </si>
   <si>
-    <t>Average alcoholic drinks per week</t>
-  </si>
-  <si>
     <t>Categorised weekly alcohol intake</t>
   </si>
   <si>
-    <t>The sum across different types of alcohol of drinks per week</t>
-  </si>
-  <si>
     <t>Townsend Deprivation Index, Quintiles</t>
   </si>
   <si>
@@ -519,10 +507,28 @@
     <t>See UKBHtn_NonCancerIllness_Mapping.xlsx for the mapping</t>
   </si>
   <si>
-    <t>Weekly METs over 150</t>
-  </si>
-  <si>
     <t>"White" and all subcategories were coded as "White", "Prefer not to answer" and unanswered were coded as "Unknown", all others were coded as "Non-white"</t>
+  </si>
+  <si>
+    <t>Average alcoholic units per week</t>
+  </si>
+  <si>
+    <t>The sum across different types of alcohol of units per week</t>
+  </si>
+  <si>
+    <t>Each type of alcohol was scaled to units according to https://www.nhs.uk/live-well/alcohol-support/calculating-alcohol-units/</t>
+  </si>
+  <si>
+    <t>METs_over600</t>
+  </si>
+  <si>
+    <t>METs_over600_</t>
+  </si>
+  <si>
+    <t>Weekly METs over 600</t>
+  </si>
+  <si>
+    <t>An indicator variable for whether the participant's weekly METs exceeded 600, the minimum threshold for WHO recommended physical activity</t>
   </si>
 </sst>
 </file>
@@ -845,237 +851,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" s="1">
         <v>21003</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1">
         <v>21003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>32</v>
@@ -1084,106 +1090,106 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1">
         <v>21000</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1">
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1">
         <v>20116</v>
@@ -1192,49 +1198,52 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
@@ -1243,18 +1252,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
@@ -1263,32 +1272,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1">
         <v>20003</v>
@@ -1297,38 +1306,38 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E25" s="1">
         <v>20003</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>35</v>
@@ -1337,35 +1346,35 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1">
         <v>2345</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E28" s="1">
         <v>20002</v>
@@ -1374,18 +1383,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" s="1">
         <v>20002</v>
@@ -1394,257 +1403,254 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E30" s="1">
         <v>21001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="1">
         <v>21001</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="C32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E32" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" t="s">
-        <v>111</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" s="1">
         <v>826</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E34" s="1">
         <v>20023</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E35" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="B36" t="s">
-        <v>118</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E36" s="1">
         <v>22040</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E37" s="1">
         <v>22040</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E38" s="1">
         <v>22040</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
         <v>117</v>
       </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E39" s="1">
         <v>1160</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B40" t="s">
+      <c r="F40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
         <v>130</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="E41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E43" s="1">
         <v>20002</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1662,229 +1668,229 @@
       <selection activeCell="A35" sqref="A35:A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>